<commit_message>
did a shit ton of analysis on fsr_S4 and made a lot of graphs
</commit_message>
<xml_diff>
--- a/data/FSR_S3/calibration/FSR_S3 Calibration Data.xlsx
+++ b/data/FSR_S3/calibration/FSR_S3 Calibration Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amro365-my.sharepoint.com/personal/pr19556_appliedmed_com/Documents/Desktop/FSR/data/FSR_S3/calibration/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickruiz/Desktop/FSR/data/FSR_S3/calibration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{10E1F4A7-3D69-9241-A771-7B59DABB1050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60E6C95E-B2F1-4F16-9A3C-15D5FC494FF9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13FDAB5E-0BE1-2742-BF5C-1C4061D65EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A44B9C34-151F-4DB5-ABDC-540135FA09DD}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="36000" windowHeight="22520" xr2:uid="{A44B9C34-151F-4DB5-ABDC-540135FA09DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>FSR</t>
   </si>
@@ -90,9 +90,6 @@
   </si>
   <si>
     <t>Applies to FSR_S3_Stability_3</t>
-  </si>
-  <si>
-    <t>y=Ax^b</t>
   </si>
 </sst>
 </file>
@@ -122,18 +119,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -148,34 +139,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -195,9 +177,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -235,7 +217,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -341,7 +323,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -483,7 +465,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -494,98 +476,98 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="3"/>
-    <col min="2" max="2" width="14.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.81640625" style="3"/>
-    <col min="6" max="6" width="8" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.81640625" style="3"/>
+    <col min="1" max="1" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="14.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.83203125" style="2"/>
+    <col min="6" max="6" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="5">
         <v>52045.263440000002</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="5">
         <v>168.34227999999999</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="5">
         <v>-1.2357800000000001</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="5">
         <v>1.8E-3</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="5">
         <v>1</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="5">
         <v>8472.7604800000008</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="6">
         <v>37255.925159999999</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="6">
         <v>144.68513999999999</v>
       </c>
       <c r="D3" s="6">
         <v>-1.1345499999999999</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="6">
         <v>2.14E-3</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="6">
         <v>1</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="6">
         <v>9007.1939700000003</v>
       </c>
       <c r="H3" s="5" t="s">
@@ -595,26 +577,26 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="6">
         <v>31615.543989999998</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="6">
         <v>149.47497999999999</v>
       </c>
       <c r="D4" s="6">
         <v>-1.08958</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="6">
         <v>2.5999999999999999E-3</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="6">
         <v>1</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="6">
         <v>11064.87717</v>
       </c>
       <c r="H4" s="5" t="s">
@@ -624,26 +606,26 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="5">
         <v>22121.195629999998</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="5">
         <v>96.616</v>
       </c>
       <c r="D5" s="5">
         <v>-0.97040000000000004</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="5">
         <v>2.3800000000000002E-3</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="5">
         <v>1</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="5">
         <v>7122.8375299999998</v>
       </c>
       <c r="H5" s="5" t="s">
@@ -653,26 +635,26 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="5">
         <v>21125.945179999999</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="5">
         <v>96.875309999999999</v>
       </c>
       <c r="D6" s="5">
         <v>-0.96352000000000004</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="5">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="5">
         <v>0.99941000000000002</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="5">
         <v>7433.6363799999999</v>
       </c>
       <c r="H6" s="5" t="s">
@@ -680,7 +662,7 @@
       </c>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -689,7 +671,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -698,7 +680,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -707,10 +689,8 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B11" s="7" t="s">
-        <v>18</v>
-      </c>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B11" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>